<commit_message>
chore/Update Thailand Flood adaptation measures in entity files
</commit_message>
<xml_diff>
--- a/requirements/adaptation_measures.xlsx
+++ b/requirements/adaptation_measures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkalomalos\Projects\unu\climada-unu\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FC3E35-3F60-413C-91CD-30A838C89ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3685AC-B6D7-436E-88A8-CBC8198EB0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -843,7 +843,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="173">
   <si>
     <t>Category_ID</t>
   </si>
@@ -1377,6 +1377,60 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>0.16 0.38 0.56</t>
+  </si>
+  <si>
+    <t>0.27 0.32 0.37</t>
+  </si>
+  <si>
+    <t>0.2 0.51 0.7</t>
+  </si>
+  <si>
+    <t>0.43 0.73 0.87</t>
+  </si>
+  <si>
+    <t>0.02 0.52 0.45</t>
+  </si>
+  <si>
+    <t>0.83 0.45 0.38</t>
+  </si>
+  <si>
+    <t>0.98 0.63 0.56</t>
+  </si>
+  <si>
+    <t>Retention reservoirs</t>
+  </si>
+  <si>
+    <t>Dredging of canals</t>
+  </si>
+  <si>
+    <t>Infiltration ponds</t>
+  </si>
+  <si>
+    <t>Recharging wells</t>
+  </si>
+  <si>
+    <t>Small dams</t>
+  </si>
+  <si>
+    <t>Τraining for agricultural topic for adaptation</t>
+  </si>
+  <si>
+    <t>Retention furrows</t>
+  </si>
+  <si>
+    <t>Improved drainage system</t>
+  </si>
+  <si>
+    <t>Agricultural zoning</t>
+  </si>
+  <si>
+    <t>Water tolerant crops</t>
+  </si>
+  <si>
+    <t>Flood index insurance</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1657,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1"/>
@@ -1667,12 +1721,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1690,7 +1745,18 @@
     <cellStyle name="Percent 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Percent 3" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
@@ -8799,1265 +8865,2052 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="36"/>
+    <col min="1" max="1" width="43.28515625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="62" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="62" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="62" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="62">
         <v>20000000</v>
       </c>
-      <c r="D2" s="36">
-        <v>1</v>
-      </c>
-      <c r="E2" s="36">
-        <v>0</v>
-      </c>
-      <c r="F2" s="36">
-        <v>0</v>
-      </c>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="62">
+        <v>1</v>
+      </c>
+      <c r="E2" s="62">
+        <v>0</v>
+      </c>
+      <c r="F2" s="62">
+        <v>0</v>
+      </c>
+      <c r="G2" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="36">
+      <c r="H2" s="62">
         <v>0.69</v>
       </c>
-      <c r="I2" s="36">
-        <v>0</v>
-      </c>
-      <c r="J2" s="36">
-        <v>1</v>
-      </c>
-      <c r="K2" s="36">
-        <v>0</v>
-      </c>
-      <c r="L2" s="36" t="s">
+      <c r="I2" s="62">
+        <v>0</v>
+      </c>
+      <c r="J2" s="62">
+        <v>1</v>
+      </c>
+      <c r="K2" s="62">
+        <v>0</v>
+      </c>
+      <c r="L2" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="36">
-        <v>0</v>
-      </c>
-      <c r="O2" s="36">
-        <v>0</v>
-      </c>
-      <c r="P2" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="36">
-        <v>1</v>
-      </c>
-      <c r="R2" s="36" t="s">
+      <c r="N2" s="62">
+        <v>0</v>
+      </c>
+      <c r="O2" s="62">
+        <v>0</v>
+      </c>
+      <c r="P2" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="62">
+        <v>1</v>
+      </c>
+      <c r="R2" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="62">
         <v>31120331.950207472</v>
       </c>
-      <c r="D3" s="36">
-        <v>1</v>
-      </c>
-      <c r="E3" s="36">
-        <v>0</v>
-      </c>
-      <c r="F3" s="36">
-        <v>0</v>
-      </c>
-      <c r="G3" s="36" t="s">
+      <c r="D3" s="62">
+        <v>1</v>
+      </c>
+      <c r="E3" s="62">
+        <v>0</v>
+      </c>
+      <c r="F3" s="62">
+        <v>0</v>
+      </c>
+      <c r="G3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="62">
         <v>0.67500000000000004</v>
       </c>
-      <c r="I3" s="36">
-        <v>0</v>
-      </c>
-      <c r="J3" s="36">
-        <v>1</v>
-      </c>
-      <c r="K3" s="36">
-        <v>0</v>
-      </c>
-      <c r="L3" s="36" t="s">
+      <c r="I3" s="62">
+        <v>0</v>
+      </c>
+      <c r="J3" s="62">
+        <v>1</v>
+      </c>
+      <c r="K3" s="62">
+        <v>0</v>
+      </c>
+      <c r="L3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="36">
-        <v>0</v>
-      </c>
-      <c r="O3" s="36">
-        <v>0</v>
-      </c>
-      <c r="P3" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="36">
-        <v>1</v>
-      </c>
-      <c r="R3" s="36" t="s">
+      <c r="N3" s="62">
+        <v>0</v>
+      </c>
+      <c r="O3" s="62">
+        <v>0</v>
+      </c>
+      <c r="P3" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="62">
+        <v>1</v>
+      </c>
+      <c r="R3" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="62">
+      <c r="C4" s="61">
         <v>1145000</v>
       </c>
-      <c r="D4" s="63">
-        <v>1</v>
-      </c>
-      <c r="E4" s="36">
-        <v>0</v>
-      </c>
-      <c r="F4" s="36">
-        <v>0</v>
-      </c>
-      <c r="G4" s="36" t="s">
+      <c r="D4" s="62">
+        <v>1</v>
+      </c>
+      <c r="E4" s="62">
+        <v>0</v>
+      </c>
+      <c r="F4" s="62">
+        <v>0</v>
+      </c>
+      <c r="G4" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="62">
         <v>0.39</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="62">
         <v>-0.05</v>
       </c>
-      <c r="J4" s="36">
-        <v>1</v>
-      </c>
-      <c r="K4" s="36">
-        <v>0</v>
-      </c>
-      <c r="L4" s="36" t="s">
+      <c r="J4" s="62">
+        <v>1</v>
+      </c>
+      <c r="K4" s="62">
+        <v>0</v>
+      </c>
+      <c r="L4" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="63" t="s">
+      <c r="M4" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="63">
-        <v>0</v>
-      </c>
-      <c r="O4" s="36">
-        <v>0</v>
-      </c>
-      <c r="P4" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="36">
-        <v>1</v>
-      </c>
-      <c r="R4" s="36" t="s">
+      <c r="N4" s="62">
+        <v>0</v>
+      </c>
+      <c r="O4" s="62">
+        <v>0</v>
+      </c>
+      <c r="P4" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="62">
+        <v>1</v>
+      </c>
+      <c r="R4" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="62" t="s">
         <v>153</v>
       </c>
       <c r="B5" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="61">
         <v>298778.18289364426</v>
       </c>
-      <c r="D5" s="63">
-        <v>1</v>
-      </c>
-      <c r="E5" s="36">
-        <v>0</v>
-      </c>
-      <c r="F5" s="36">
-        <v>0</v>
-      </c>
-      <c r="G5" s="36" t="s">
+      <c r="D5" s="62">
+        <v>1</v>
+      </c>
+      <c r="E5" s="62">
+        <v>0</v>
+      </c>
+      <c r="F5" s="62">
+        <v>0</v>
+      </c>
+      <c r="G5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="62">
         <v>0.75</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="62">
         <v>0.06</v>
       </c>
-      <c r="J5" s="36">
-        <v>1</v>
-      </c>
-      <c r="K5" s="36">
-        <v>0</v>
-      </c>
-      <c r="L5" s="36" t="s">
+      <c r="J5" s="62">
+        <v>1</v>
+      </c>
+      <c r="K5" s="62">
+        <v>0</v>
+      </c>
+      <c r="L5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="63">
-        <v>0</v>
-      </c>
-      <c r="O5" s="36">
-        <v>0</v>
-      </c>
-      <c r="P5" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="36">
-        <v>1</v>
-      </c>
-      <c r="R5" s="36" t="s">
+      <c r="N5" s="62">
+        <v>0</v>
+      </c>
+      <c r="O5" s="62">
+        <v>0</v>
+      </c>
+      <c r="P5" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="62">
+        <v>1</v>
+      </c>
+      <c r="R5" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="62">
         <v>22370744.852031101</v>
       </c>
-      <c r="D6" s="36">
-        <v>1</v>
-      </c>
-      <c r="E6" s="36">
-        <v>0</v>
-      </c>
-      <c r="F6" s="36">
-        <v>0</v>
-      </c>
-      <c r="G6" s="36" t="s">
+      <c r="D6" s="62">
+        <v>1</v>
+      </c>
+      <c r="E6" s="62">
+        <v>0</v>
+      </c>
+      <c r="F6" s="62">
+        <v>0</v>
+      </c>
+      <c r="G6" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="62">
         <v>0.78</v>
       </c>
-      <c r="I6" s="36">
-        <v>0</v>
-      </c>
-      <c r="J6" s="36">
-        <v>1</v>
-      </c>
-      <c r="K6" s="36">
-        <v>0</v>
-      </c>
-      <c r="L6" s="36" t="s">
+      <c r="I6" s="62">
+        <v>0</v>
+      </c>
+      <c r="J6" s="62">
+        <v>1</v>
+      </c>
+      <c r="K6" s="62">
+        <v>0</v>
+      </c>
+      <c r="L6" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="36">
-        <v>0</v>
-      </c>
-      <c r="O6" s="36">
-        <v>0</v>
-      </c>
-      <c r="P6" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="36">
-        <v>1</v>
-      </c>
-      <c r="R6" s="36" t="s">
+      <c r="N6" s="62">
+        <v>0</v>
+      </c>
+      <c r="O6" s="62">
+        <v>0</v>
+      </c>
+      <c r="P6" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="62">
+        <v>1</v>
+      </c>
+      <c r="R6" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="62">
         <v>35952982.797907144</v>
       </c>
-      <c r="D7" s="36">
-        <v>1</v>
-      </c>
-      <c r="E7" s="36">
-        <v>0</v>
-      </c>
-      <c r="F7" s="36">
-        <v>0</v>
-      </c>
-      <c r="G7" s="36" t="s">
+      <c r="D7" s="62">
+        <v>1</v>
+      </c>
+      <c r="E7" s="62">
+        <v>0</v>
+      </c>
+      <c r="F7" s="62">
+        <v>0</v>
+      </c>
+      <c r="G7" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="62">
         <v>0.75</v>
       </c>
-      <c r="I7" s="36">
-        <v>0</v>
-      </c>
-      <c r="J7" s="36">
-        <v>1</v>
-      </c>
-      <c r="K7" s="36">
-        <v>0</v>
-      </c>
-      <c r="L7" s="36" t="s">
+      <c r="I7" s="62">
+        <v>0</v>
+      </c>
+      <c r="J7" s="62">
+        <v>1</v>
+      </c>
+      <c r="K7" s="62">
+        <v>0</v>
+      </c>
+      <c r="L7" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="M7" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="36">
-        <v>0</v>
-      </c>
-      <c r="O7" s="36">
-        <v>0</v>
-      </c>
-      <c r="P7" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="36">
-        <v>1</v>
-      </c>
-      <c r="R7" s="36" t="s">
+      <c r="N7" s="62">
+        <v>0</v>
+      </c>
+      <c r="O7" s="62">
+        <v>0</v>
+      </c>
+      <c r="P7" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="62">
+        <v>1</v>
+      </c>
+      <c r="R7" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="62">
         <v>34035490.382018767</v>
       </c>
-      <c r="D8" s="36">
-        <v>1</v>
-      </c>
-      <c r="E8" s="36">
-        <v>0</v>
-      </c>
-      <c r="F8" s="36">
-        <v>0</v>
-      </c>
-      <c r="G8" s="36" t="s">
+      <c r="D8" s="62">
+        <v>1</v>
+      </c>
+      <c r="E8" s="62">
+        <v>0</v>
+      </c>
+      <c r="F8" s="62">
+        <v>0</v>
+      </c>
+      <c r="G8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="62">
         <v>0.8</v>
       </c>
-      <c r="I8" s="36">
-        <v>0</v>
-      </c>
-      <c r="J8" s="36">
-        <v>1</v>
-      </c>
-      <c r="K8" s="36">
-        <v>0</v>
-      </c>
-      <c r="L8" s="36" t="s">
+      <c r="I8" s="62">
+        <v>0</v>
+      </c>
+      <c r="J8" s="62">
+        <v>1</v>
+      </c>
+      <c r="K8" s="62">
+        <v>0</v>
+      </c>
+      <c r="L8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="36">
-        <v>0</v>
-      </c>
-      <c r="O8" s="36">
-        <v>0</v>
-      </c>
-      <c r="P8" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="36">
-        <v>1</v>
-      </c>
-      <c r="R8" s="36" t="s">
+      <c r="N8" s="62">
+        <v>0</v>
+      </c>
+      <c r="O8" s="62">
+        <v>0</v>
+      </c>
+      <c r="P8" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="62">
+        <v>1</v>
+      </c>
+      <c r="R8" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="62">
         <v>22398708.28309615</v>
       </c>
-      <c r="D9" s="36">
-        <v>1</v>
-      </c>
-      <c r="E9" s="36">
-        <v>0</v>
-      </c>
-      <c r="F9" s="36">
-        <v>0</v>
-      </c>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="62">
+        <v>1</v>
+      </c>
+      <c r="E9" s="62">
+        <v>0</v>
+      </c>
+      <c r="F9" s="62">
+        <v>0</v>
+      </c>
+      <c r="G9" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="62">
         <v>0.67998999999999998</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="62">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J9" s="36">
-        <v>1</v>
-      </c>
-      <c r="K9" s="36">
-        <v>0</v>
-      </c>
-      <c r="L9" s="36" t="s">
+      <c r="J9" s="62">
+        <v>1</v>
+      </c>
+      <c r="K9" s="62">
+        <v>0</v>
+      </c>
+      <c r="L9" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="36">
-        <v>0</v>
-      </c>
-      <c r="O9" s="36">
-        <v>0</v>
-      </c>
-      <c r="P9" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="36">
-        <v>1</v>
-      </c>
-      <c r="R9" s="36" t="s">
+      <c r="N9" s="62">
+        <v>0</v>
+      </c>
+      <c r="O9" s="62">
+        <v>0</v>
+      </c>
+      <c r="P9" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="62">
+        <v>1</v>
+      </c>
+      <c r="R9" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="62">
         <v>113132052.53741448</v>
       </c>
-      <c r="D10" s="36">
-        <v>1</v>
-      </c>
-      <c r="E10" s="36">
-        <v>0</v>
-      </c>
-      <c r="F10" s="36">
-        <v>0</v>
-      </c>
-      <c r="G10" s="36" t="s">
+      <c r="D10" s="62">
+        <v>1</v>
+      </c>
+      <c r="E10" s="62">
+        <v>0</v>
+      </c>
+      <c r="F10" s="62">
+        <v>0</v>
+      </c>
+      <c r="G10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="62">
         <v>0.6</v>
       </c>
-      <c r="I10" s="36">
-        <v>0</v>
-      </c>
-      <c r="J10" s="36">
-        <v>1</v>
-      </c>
-      <c r="K10" s="36">
-        <v>0</v>
-      </c>
-      <c r="L10" s="36" t="s">
+      <c r="I10" s="62">
+        <v>0</v>
+      </c>
+      <c r="J10" s="62">
+        <v>1</v>
+      </c>
+      <c r="K10" s="62">
+        <v>0</v>
+      </c>
+      <c r="L10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="36">
-        <v>0</v>
-      </c>
-      <c r="O10" s="36">
-        <v>0</v>
-      </c>
-      <c r="P10" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="36">
-        <v>1</v>
-      </c>
-      <c r="R10" s="36" t="s">
+      <c r="N10" s="62">
+        <v>0</v>
+      </c>
+      <c r="O10" s="62">
+        <v>0</v>
+      </c>
+      <c r="P10" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="62">
+        <v>1</v>
+      </c>
+      <c r="R10" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="62">
         <v>196542972.62855905</v>
       </c>
-      <c r="D11" s="36">
-        <v>1</v>
-      </c>
-      <c r="E11" s="36">
-        <v>0</v>
-      </c>
-      <c r="F11" s="36">
-        <v>0</v>
-      </c>
-      <c r="G11" s="36" t="s">
+      <c r="D11" s="62">
+        <v>1</v>
+      </c>
+      <c r="E11" s="62">
+        <v>0</v>
+      </c>
+      <c r="F11" s="62">
+        <v>0</v>
+      </c>
+      <c r="G11" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="62">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I11" s="36">
-        <v>0</v>
-      </c>
-      <c r="J11" s="36">
-        <v>1</v>
-      </c>
-      <c r="K11" s="36">
-        <v>0</v>
-      </c>
-      <c r="L11" s="36" t="s">
+      <c r="I11" s="62">
+        <v>0</v>
+      </c>
+      <c r="J11" s="62">
+        <v>1</v>
+      </c>
+      <c r="K11" s="62">
+        <v>0</v>
+      </c>
+      <c r="L11" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="36">
-        <v>0</v>
-      </c>
-      <c r="O11" s="36">
-        <v>0</v>
-      </c>
-      <c r="P11" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="36">
-        <v>1</v>
-      </c>
-      <c r="R11" s="36" t="s">
+      <c r="N11" s="62">
+        <v>0</v>
+      </c>
+      <c r="O11" s="62">
+        <v>0</v>
+      </c>
+      <c r="P11" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="62">
+        <v>1</v>
+      </c>
+      <c r="R11" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="62">
         <v>3600000</v>
       </c>
-      <c r="D12" s="36">
-        <v>1</v>
-      </c>
-      <c r="E12" s="36">
-        <v>0</v>
-      </c>
-      <c r="F12" s="36">
-        <v>0</v>
-      </c>
-      <c r="G12" s="36" t="s">
+      <c r="D12" s="62">
+        <v>1</v>
+      </c>
+      <c r="E12" s="62">
+        <v>0</v>
+      </c>
+      <c r="F12" s="62">
+        <v>0</v>
+      </c>
+      <c r="G12" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="62">
         <v>0.69</v>
       </c>
-      <c r="I12" s="36">
-        <v>0</v>
-      </c>
-      <c r="J12" s="36">
-        <v>1</v>
-      </c>
-      <c r="K12" s="36">
-        <v>0</v>
-      </c>
-      <c r="L12" s="36" t="s">
+      <c r="I12" s="62">
+        <v>0</v>
+      </c>
+      <c r="J12" s="62">
+        <v>1</v>
+      </c>
+      <c r="K12" s="62">
+        <v>0</v>
+      </c>
+      <c r="L12" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M12" s="36" t="s">
+      <c r="M12" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="36">
-        <v>0</v>
-      </c>
-      <c r="O12" s="36">
-        <v>0</v>
-      </c>
-      <c r="P12" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="36">
-        <v>1</v>
-      </c>
-      <c r="R12" s="36" t="s">
+      <c r="N12" s="62">
+        <v>0</v>
+      </c>
+      <c r="O12" s="62">
+        <v>0</v>
+      </c>
+      <c r="P12" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="62">
+        <v>1</v>
+      </c>
+      <c r="R12" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="62">
         <v>5601659.7510373443</v>
       </c>
-      <c r="D13" s="36">
-        <v>1</v>
-      </c>
-      <c r="E13" s="36">
-        <v>0</v>
-      </c>
-      <c r="F13" s="36">
-        <v>0</v>
-      </c>
-      <c r="G13" s="36" t="s">
+      <c r="D13" s="62">
+        <v>1</v>
+      </c>
+      <c r="E13" s="62">
+        <v>0</v>
+      </c>
+      <c r="F13" s="62">
+        <v>0</v>
+      </c>
+      <c r="G13" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="62">
         <v>0.67500000000000004</v>
       </c>
-      <c r="I13" s="36">
-        <v>0</v>
-      </c>
-      <c r="J13" s="36">
-        <v>1</v>
-      </c>
-      <c r="K13" s="36">
-        <v>0</v>
-      </c>
-      <c r="L13" s="36" t="s">
+      <c r="I13" s="62">
+        <v>0</v>
+      </c>
+      <c r="J13" s="62">
+        <v>1</v>
+      </c>
+      <c r="K13" s="62">
+        <v>0</v>
+      </c>
+      <c r="L13" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="36" t="s">
+      <c r="M13" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N13" s="36">
-        <v>0</v>
-      </c>
-      <c r="O13" s="36">
-        <v>0</v>
-      </c>
-      <c r="P13" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="36">
-        <v>1</v>
-      </c>
-      <c r="R13" s="36" t="s">
+      <c r="N13" s="62">
+        <v>0</v>
+      </c>
+      <c r="O13" s="62">
+        <v>0</v>
+      </c>
+      <c r="P13" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="62">
+        <v>1</v>
+      </c>
+      <c r="R13" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="62">
         <v>4026734.073365598</v>
       </c>
-      <c r="D14" s="36">
-        <v>1</v>
-      </c>
-      <c r="E14" s="36">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36">
-        <v>0</v>
-      </c>
-      <c r="G14" s="36" t="s">
+      <c r="D14" s="62">
+        <v>1</v>
+      </c>
+      <c r="E14" s="62">
+        <v>0</v>
+      </c>
+      <c r="F14" s="62">
+        <v>0</v>
+      </c>
+      <c r="G14" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="62">
         <v>0.78</v>
       </c>
-      <c r="I14" s="36">
-        <v>0</v>
-      </c>
-      <c r="J14" s="36">
-        <v>1</v>
-      </c>
-      <c r="K14" s="36">
-        <v>0</v>
-      </c>
-      <c r="L14" s="36" t="s">
+      <c r="I14" s="62">
+        <v>0</v>
+      </c>
+      <c r="J14" s="62">
+        <v>1</v>
+      </c>
+      <c r="K14" s="62">
+        <v>0</v>
+      </c>
+      <c r="L14" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="36" t="s">
+      <c r="M14" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="36">
-        <v>0</v>
-      </c>
-      <c r="O14" s="36">
-        <v>0</v>
-      </c>
-      <c r="P14" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="36">
-        <v>1</v>
-      </c>
-      <c r="R14" s="36" t="s">
+      <c r="N14" s="62">
+        <v>0</v>
+      </c>
+      <c r="O14" s="62">
+        <v>0</v>
+      </c>
+      <c r="P14" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="62">
+        <v>1</v>
+      </c>
+      <c r="R14" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="62">
         <v>35377735.073140629</v>
       </c>
-      <c r="D15" s="36">
-        <v>1</v>
-      </c>
-      <c r="E15" s="36">
-        <v>0</v>
-      </c>
-      <c r="F15" s="36">
-        <v>0</v>
-      </c>
-      <c r="G15" s="36" t="s">
+      <c r="D15" s="62">
+        <v>1</v>
+      </c>
+      <c r="E15" s="62">
+        <v>0</v>
+      </c>
+      <c r="F15" s="62">
+        <v>0</v>
+      </c>
+      <c r="G15" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="62">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I15" s="36">
-        <v>0</v>
-      </c>
-      <c r="J15" s="36">
-        <v>1</v>
-      </c>
-      <c r="K15" s="36">
-        <v>0</v>
-      </c>
-      <c r="L15" s="36" t="s">
+      <c r="I15" s="62">
+        <v>0</v>
+      </c>
+      <c r="J15" s="62">
+        <v>1</v>
+      </c>
+      <c r="K15" s="62">
+        <v>0</v>
+      </c>
+      <c r="L15" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="36">
-        <v>0</v>
-      </c>
-      <c r="O15" s="36">
-        <v>0</v>
-      </c>
-      <c r="P15" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="36">
-        <v>1</v>
-      </c>
-      <c r="R15" s="36" t="s">
+      <c r="N15" s="62">
+        <v>0</v>
+      </c>
+      <c r="O15" s="62">
+        <v>0</v>
+      </c>
+      <c r="P15" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="62">
+        <v>1</v>
+      </c>
+      <c r="R15" s="62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="62">
         <v>3021000</v>
       </c>
-      <c r="D16" s="36">
-        <v>1</v>
-      </c>
-      <c r="E16" s="36">
-        <v>0</v>
-      </c>
-      <c r="F16" s="36">
-        <v>0</v>
-      </c>
-      <c r="G16" s="36" t="s">
+      <c r="D16" s="62">
+        <v>1</v>
+      </c>
+      <c r="E16" s="62">
+        <v>0</v>
+      </c>
+      <c r="F16" s="62">
+        <v>0</v>
+      </c>
+      <c r="G16" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="62">
         <v>0.65</v>
       </c>
-      <c r="I16" s="36">
-        <v>0</v>
-      </c>
-      <c r="J16" s="36">
-        <v>1</v>
-      </c>
-      <c r="K16" s="36">
-        <v>0</v>
-      </c>
-      <c r="L16" s="36" t="s">
+      <c r="I16" s="62">
+        <v>0</v>
+      </c>
+      <c r="J16" s="62">
+        <v>1</v>
+      </c>
+      <c r="K16" s="62">
+        <v>0</v>
+      </c>
+      <c r="L16" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="36">
-        <v>0</v>
-      </c>
-      <c r="O16" s="36">
-        <v>0</v>
-      </c>
-      <c r="P16" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="36">
-        <v>1</v>
-      </c>
-      <c r="R16" s="36" t="s">
+      <c r="N16" s="62">
+        <v>0</v>
+      </c>
+      <c r="O16" s="62">
+        <v>0</v>
+      </c>
+      <c r="P16" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="62">
+        <v>1</v>
+      </c>
+      <c r="R16" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="62">
         <v>6616532.7210103311</v>
       </c>
-      <c r="D17" s="36">
-        <v>1</v>
-      </c>
-      <c r="E17" s="36">
-        <v>0</v>
-      </c>
-      <c r="F17" s="36">
-        <v>0</v>
-      </c>
-      <c r="G17" s="36" t="s">
+      <c r="D17" s="62">
+        <v>1</v>
+      </c>
+      <c r="E17" s="62">
+        <v>0</v>
+      </c>
+      <c r="F17" s="62">
+        <v>0</v>
+      </c>
+      <c r="G17" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="62">
         <v>0.6</v>
       </c>
-      <c r="I17" s="36">
-        <v>0</v>
-      </c>
-      <c r="J17" s="36">
-        <v>1</v>
-      </c>
-      <c r="K17" s="36">
-        <v>0</v>
-      </c>
-      <c r="L17" s="36" t="s">
+      <c r="I17" s="62">
+        <v>0</v>
+      </c>
+      <c r="J17" s="62">
+        <v>1</v>
+      </c>
+      <c r="K17" s="62">
+        <v>0</v>
+      </c>
+      <c r="L17" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="36">
-        <v>0</v>
-      </c>
-      <c r="O17" s="36">
-        <v>0</v>
-      </c>
-      <c r="P17" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="36">
-        <v>1</v>
-      </c>
-      <c r="R17" s="36" t="s">
+      <c r="N17" s="62">
+        <v>0</v>
+      </c>
+      <c r="O17" s="62">
+        <v>0</v>
+      </c>
+      <c r="P17" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="62">
+        <v>1</v>
+      </c>
+      <c r="R17" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="62">
         <v>3777900</v>
       </c>
-      <c r="D18" s="36">
-        <v>1</v>
-      </c>
-      <c r="E18" s="36">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <v>0</v>
-      </c>
-      <c r="G18" s="36" t="s">
+      <c r="D18" s="62">
+        <v>1</v>
+      </c>
+      <c r="E18" s="62">
+        <v>0</v>
+      </c>
+      <c r="F18" s="62">
+        <v>0</v>
+      </c>
+      <c r="G18" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="62">
         <v>0.7</v>
       </c>
-      <c r="I18" s="36">
-        <v>0</v>
-      </c>
-      <c r="J18" s="36">
-        <v>1</v>
-      </c>
-      <c r="K18" s="36">
-        <v>0</v>
-      </c>
-      <c r="L18" s="36" t="s">
+      <c r="I18" s="62">
+        <v>0</v>
+      </c>
+      <c r="J18" s="62">
+        <v>1</v>
+      </c>
+      <c r="K18" s="62">
+        <v>0</v>
+      </c>
+      <c r="L18" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="36">
-        <v>0</v>
-      </c>
-      <c r="O18" s="36">
-        <v>0</v>
-      </c>
-      <c r="P18" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="36">
-        <v>1</v>
-      </c>
-      <c r="R18" s="36" t="s">
+      <c r="N18" s="62">
+        <v>0</v>
+      </c>
+      <c r="O18" s="62">
+        <v>0</v>
+      </c>
+      <c r="P18" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="62">
+        <v>1</v>
+      </c>
+      <c r="R18" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="62">
         <v>13233065.442020662</v>
       </c>
-      <c r="D19" s="36">
-        <v>1</v>
-      </c>
-      <c r="E19" s="36">
-        <v>0</v>
-      </c>
-      <c r="F19" s="36">
-        <v>0</v>
-      </c>
-      <c r="G19" s="36" t="s">
+      <c r="D19" s="62">
+        <v>1</v>
+      </c>
+      <c r="E19" s="62">
+        <v>0</v>
+      </c>
+      <c r="F19" s="62">
+        <v>0</v>
+      </c>
+      <c r="G19" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="62">
         <v>0.52</v>
       </c>
-      <c r="I19" s="36">
-        <v>0</v>
-      </c>
-      <c r="J19" s="36">
-        <v>1</v>
-      </c>
-      <c r="K19" s="36">
-        <v>0</v>
-      </c>
-      <c r="L19" s="36" t="s">
+      <c r="I19" s="62">
+        <v>0</v>
+      </c>
+      <c r="J19" s="62">
+        <v>1</v>
+      </c>
+      <c r="K19" s="62">
+        <v>0</v>
+      </c>
+      <c r="L19" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M19" s="36" t="s">
+      <c r="M19" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N19" s="36">
-        <v>0</v>
-      </c>
-      <c r="O19" s="36">
-        <v>0</v>
-      </c>
-      <c r="P19" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="36">
-        <v>1</v>
-      </c>
-      <c r="R19" s="36" t="s">
+      <c r="N19" s="62">
+        <v>0</v>
+      </c>
+      <c r="O19" s="62">
+        <v>0</v>
+      </c>
+      <c r="P19" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="62">
+        <v>1</v>
+      </c>
+      <c r="R19" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="62">
         <v>12870471.774193544</v>
       </c>
-      <c r="D20" s="36">
-        <v>1</v>
-      </c>
-      <c r="E20" s="36">
-        <v>0</v>
-      </c>
-      <c r="F20" s="36">
-        <v>0</v>
-      </c>
-      <c r="G20" s="36" t="s">
+      <c r="D20" s="62">
+        <v>1</v>
+      </c>
+      <c r="E20" s="62">
+        <v>0</v>
+      </c>
+      <c r="F20" s="62">
+        <v>0</v>
+      </c>
+      <c r="G20" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="62">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I20" s="36">
-        <v>0</v>
-      </c>
-      <c r="J20" s="36">
-        <v>1</v>
-      </c>
-      <c r="K20" s="36">
-        <v>0</v>
-      </c>
-      <c r="L20" s="36" t="s">
+      <c r="I20" s="62">
+        <v>0</v>
+      </c>
+      <c r="J20" s="62">
+        <v>1</v>
+      </c>
+      <c r="K20" s="62">
+        <v>0</v>
+      </c>
+      <c r="L20" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="M20" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N20" s="36">
-        <v>0</v>
-      </c>
-      <c r="O20" s="36">
-        <v>0</v>
-      </c>
-      <c r="P20" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="36">
-        <v>1</v>
-      </c>
-      <c r="R20" s="36" t="s">
+      <c r="N20" s="62">
+        <v>0</v>
+      </c>
+      <c r="O20" s="62">
+        <v>0</v>
+      </c>
+      <c r="P20" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="62">
+        <v>1</v>
+      </c>
+      <c r="R20" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="62">
         <v>21420000</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="62">
         <v>0.75</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="62">
         <v>0.75</v>
       </c>
-      <c r="F21" s="36">
-        <v>0</v>
-      </c>
-      <c r="G21" s="36" t="s">
+      <c r="F21" s="62">
+        <v>0</v>
+      </c>
+      <c r="G21" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="62">
         <v>0.45</v>
       </c>
-      <c r="I21" s="36">
-        <v>0</v>
-      </c>
-      <c r="J21" s="36">
-        <v>1</v>
-      </c>
-      <c r="K21" s="36">
-        <v>0</v>
-      </c>
-      <c r="L21" s="36" t="s">
+      <c r="I21" s="62">
+        <v>0</v>
+      </c>
+      <c r="J21" s="62">
+        <v>1</v>
+      </c>
+      <c r="K21" s="62">
+        <v>0</v>
+      </c>
+      <c r="L21" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="36">
-        <v>0</v>
-      </c>
-      <c r="O21" s="36">
-        <v>0</v>
-      </c>
-      <c r="P21" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="36">
-        <v>1</v>
-      </c>
-      <c r="R21" s="36" t="s">
+      <c r="N21" s="62">
+        <v>0</v>
+      </c>
+      <c r="O21" s="62">
+        <v>0</v>
+      </c>
+      <c r="P21" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="62">
+        <v>1</v>
+      </c>
+      <c r="R21" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="62">
         <v>105000000</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="62">
         <v>0.75</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="62">
         <v>0.75</v>
       </c>
-      <c r="F22" s="36">
-        <v>0</v>
-      </c>
-      <c r="G22" s="36" t="s">
+      <c r="F22" s="62">
+        <v>0</v>
+      </c>
+      <c r="G22" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="62">
         <v>0.47</v>
       </c>
-      <c r="I22" s="36">
-        <v>0</v>
-      </c>
-      <c r="J22" s="36">
-        <v>1</v>
-      </c>
-      <c r="K22" s="36">
-        <v>0</v>
-      </c>
-      <c r="L22" s="36" t="s">
+      <c r="I22" s="62">
+        <v>0</v>
+      </c>
+      <c r="J22" s="62">
+        <v>1</v>
+      </c>
+      <c r="K22" s="62">
+        <v>0</v>
+      </c>
+      <c r="L22" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="36">
-        <v>0</v>
-      </c>
-      <c r="O22" s="36">
-        <v>0</v>
-      </c>
-      <c r="P22" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="36">
-        <v>1</v>
-      </c>
-      <c r="R22" s="36" t="s">
+      <c r="N22" s="62">
+        <v>0</v>
+      </c>
+      <c r="O22" s="62">
+        <v>0</v>
+      </c>
+      <c r="P22" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="62">
+        <v>1</v>
+      </c>
+      <c r="R22" s="62" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="61">
+        <v>69156293.222683266</v>
+      </c>
+      <c r="D23" s="62">
+        <v>1</v>
+      </c>
+      <c r="E23" s="62">
+        <v>0</v>
+      </c>
+      <c r="F23" s="62">
+        <v>0</v>
+      </c>
+      <c r="G23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="62">
+        <v>0.35</v>
+      </c>
+      <c r="I23" s="62">
+        <v>0</v>
+      </c>
+      <c r="J23" s="62">
+        <v>1</v>
+      </c>
+      <c r="K23" s="62">
+        <v>0</v>
+      </c>
+      <c r="L23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" s="62">
+        <v>0</v>
+      </c>
+      <c r="O23" s="62">
+        <v>0</v>
+      </c>
+      <c r="P23" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="62">
+        <v>1</v>
+      </c>
+      <c r="R23" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="61">
+        <v>10653600</v>
+      </c>
+      <c r="D24" s="62">
+        <v>1</v>
+      </c>
+      <c r="E24" s="62">
+        <v>0</v>
+      </c>
+      <c r="F24" s="62">
+        <v>0</v>
+      </c>
+      <c r="G24" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="62">
+        <v>0.85</v>
+      </c>
+      <c r="I24" s="62">
+        <v>0</v>
+      </c>
+      <c r="J24" s="62">
+        <v>1</v>
+      </c>
+      <c r="K24" s="62">
+        <v>0</v>
+      </c>
+      <c r="L24" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N24" s="62">
+        <v>0</v>
+      </c>
+      <c r="O24" s="62">
+        <v>0</v>
+      </c>
+      <c r="P24" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="62">
+        <v>1</v>
+      </c>
+      <c r="R24" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="61">
+        <v>40341171.046565235</v>
+      </c>
+      <c r="D25" s="62">
+        <v>1</v>
+      </c>
+      <c r="E25" s="62">
+        <v>0</v>
+      </c>
+      <c r="F25" s="62">
+        <v>0</v>
+      </c>
+      <c r="G25" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="62">
+        <v>0.6</v>
+      </c>
+      <c r="I25" s="62">
+        <v>0</v>
+      </c>
+      <c r="J25" s="62">
+        <v>1</v>
+      </c>
+      <c r="K25" s="62">
+        <v>0</v>
+      </c>
+      <c r="L25" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" s="62">
+        <v>0</v>
+      </c>
+      <c r="O25" s="62">
+        <v>0</v>
+      </c>
+      <c r="P25" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="62">
+        <v>1</v>
+      </c>
+      <c r="R25" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="61">
+        <v>52523956.178019531</v>
+      </c>
+      <c r="D26" s="62">
+        <v>1</v>
+      </c>
+      <c r="E26" s="62">
+        <v>0</v>
+      </c>
+      <c r="F26" s="62">
+        <v>0</v>
+      </c>
+      <c r="G26" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="62">
+        <v>0.52</v>
+      </c>
+      <c r="I26" s="62">
+        <v>0</v>
+      </c>
+      <c r="J26" s="62">
+        <v>1</v>
+      </c>
+      <c r="K26" s="62">
+        <v>0</v>
+      </c>
+      <c r="L26" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="62">
+        <v>0</v>
+      </c>
+      <c r="O26" s="62">
+        <v>0</v>
+      </c>
+      <c r="P26" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="62">
+        <v>1</v>
+      </c>
+      <c r="R26" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="61">
+        <v>77706469.3767436</v>
+      </c>
+      <c r="D27" s="62">
+        <v>1</v>
+      </c>
+      <c r="E27" s="62">
+        <v>0</v>
+      </c>
+      <c r="F27" s="62">
+        <v>0</v>
+      </c>
+      <c r="G27" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="62">
+        <v>0.35</v>
+      </c>
+      <c r="I27" s="62">
+        <v>0</v>
+      </c>
+      <c r="J27" s="62">
+        <v>1</v>
+      </c>
+      <c r="K27" s="62">
+        <v>0</v>
+      </c>
+      <c r="L27" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="62">
+        <v>0</v>
+      </c>
+      <c r="O27" s="62">
+        <v>0</v>
+      </c>
+      <c r="P27" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="62">
+        <v>1</v>
+      </c>
+      <c r="R27" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="61">
+        <v>168148056.37771592</v>
+      </c>
+      <c r="D28" s="62">
+        <v>1</v>
+      </c>
+      <c r="E28" s="62">
+        <v>0</v>
+      </c>
+      <c r="F28" s="62">
+        <v>0</v>
+      </c>
+      <c r="G28" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="62">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I28" s="62">
+        <v>0</v>
+      </c>
+      <c r="J28" s="62">
+        <v>1</v>
+      </c>
+      <c r="K28" s="62">
+        <v>0</v>
+      </c>
+      <c r="L28" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="62">
+        <v>0</v>
+      </c>
+      <c r="O28" s="62">
+        <v>0</v>
+      </c>
+      <c r="P28" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="62">
+        <v>1</v>
+      </c>
+      <c r="R28" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="61">
+        <v>459403.00584958051</v>
+      </c>
+      <c r="D29" s="62">
+        <v>1</v>
+      </c>
+      <c r="E29" s="62">
+        <v>0</v>
+      </c>
+      <c r="F29" s="62">
+        <v>0</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="62">
+        <v>0.995</v>
+      </c>
+      <c r="I29" s="62">
+        <v>0</v>
+      </c>
+      <c r="J29" s="62">
+        <v>1</v>
+      </c>
+      <c r="K29" s="62">
+        <v>0</v>
+      </c>
+      <c r="L29" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="62">
+        <v>0</v>
+      </c>
+      <c r="O29" s="62">
+        <v>0</v>
+      </c>
+      <c r="P29" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="62">
+        <v>1</v>
+      </c>
+      <c r="R29" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="61">
+        <v>3021000</v>
+      </c>
+      <c r="D30" s="62">
+        <v>1</v>
+      </c>
+      <c r="E30" s="62">
+        <v>0</v>
+      </c>
+      <c r="F30" s="62">
+        <v>0</v>
+      </c>
+      <c r="G30" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="62">
+        <v>0.98</v>
+      </c>
+      <c r="I30" s="62">
+        <v>0</v>
+      </c>
+      <c r="J30" s="62">
+        <v>1</v>
+      </c>
+      <c r="K30" s="62">
+        <v>0</v>
+      </c>
+      <c r="L30" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N30" s="62">
+        <v>0</v>
+      </c>
+      <c r="O30" s="62">
+        <v>0</v>
+      </c>
+      <c r="P30" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="62">
+        <v>1</v>
+      </c>
+      <c r="R30" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="61">
+        <v>21895243.97692433</v>
+      </c>
+      <c r="D31" s="62">
+        <v>1</v>
+      </c>
+      <c r="E31" s="62">
+        <v>0</v>
+      </c>
+      <c r="F31" s="62">
+        <v>0</v>
+      </c>
+      <c r="G31" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="62">
+        <v>0.97</v>
+      </c>
+      <c r="I31" s="62">
+        <v>0</v>
+      </c>
+      <c r="J31" s="62">
+        <v>1</v>
+      </c>
+      <c r="K31" s="62">
+        <v>0</v>
+      </c>
+      <c r="L31" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" s="62">
+        <v>0</v>
+      </c>
+      <c r="O31" s="62">
+        <v>0</v>
+      </c>
+      <c r="P31" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="62">
+        <v>1</v>
+      </c>
+      <c r="R31" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="61">
+        <v>1620000</v>
+      </c>
+      <c r="D32" s="62">
+        <v>1</v>
+      </c>
+      <c r="E32" s="62">
+        <v>0</v>
+      </c>
+      <c r="F32" s="62">
+        <v>0</v>
+      </c>
+      <c r="G32" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="62">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I32" s="62">
+        <v>0</v>
+      </c>
+      <c r="J32" s="62">
+        <v>1</v>
+      </c>
+      <c r="K32" s="62">
+        <v>0</v>
+      </c>
+      <c r="L32" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="62">
+        <v>0</v>
+      </c>
+      <c r="O32" s="62">
+        <v>0</v>
+      </c>
+      <c r="P32" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="62">
+        <v>1</v>
+      </c>
+      <c r="R32" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="61">
+        <v>30674921.313818198</v>
+      </c>
+      <c r="D33" s="62">
+        <v>1</v>
+      </c>
+      <c r="E33" s="62">
+        <v>0</v>
+      </c>
+      <c r="F33" s="62">
+        <v>0</v>
+      </c>
+      <c r="G33" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="62">
+        <v>0.9</v>
+      </c>
+      <c r="I33" s="62">
+        <v>0</v>
+      </c>
+      <c r="J33" s="62">
+        <v>1</v>
+      </c>
+      <c r="K33" s="62">
+        <v>0</v>
+      </c>
+      <c r="L33" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="62">
+        <v>0</v>
+      </c>
+      <c r="O33" s="62">
+        <v>0</v>
+      </c>
+      <c r="P33" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="62">
+        <v>1</v>
+      </c>
+      <c r="R33" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="61">
+        <v>13500000</v>
+      </c>
+      <c r="D34" s="62">
+        <v>1</v>
+      </c>
+      <c r="E34" s="62">
+        <v>0</v>
+      </c>
+      <c r="F34" s="62">
+        <v>0</v>
+      </c>
+      <c r="G34" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="62">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="I34" s="62">
+        <v>0</v>
+      </c>
+      <c r="J34" s="62">
+        <v>1</v>
+      </c>
+      <c r="K34" s="62">
+        <v>0</v>
+      </c>
+      <c r="L34" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="62">
+        <v>0</v>
+      </c>
+      <c r="O34" s="62">
+        <v>0</v>
+      </c>
+      <c r="P34" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="62">
+        <v>1</v>
+      </c>
+      <c r="R34" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="B35" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="61">
+        <v>13500000</v>
+      </c>
+      <c r="D35" s="62">
+        <v>1</v>
+      </c>
+      <c r="E35" s="62">
+        <v>0</v>
+      </c>
+      <c r="F35" s="62">
+        <v>0</v>
+      </c>
+      <c r="G35" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="62">
+        <v>0.98</v>
+      </c>
+      <c r="I35" s="62">
+        <v>0</v>
+      </c>
+      <c r="J35" s="62">
+        <v>1</v>
+      </c>
+      <c r="K35" s="62">
+        <v>0</v>
+      </c>
+      <c r="L35" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N35" s="62">
+        <v>0</v>
+      </c>
+      <c r="O35" s="62">
+        <v>0</v>
+      </c>
+      <c r="P35" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="62">
+        <v>1</v>
+      </c>
+      <c r="R35" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="61">
+        <v>92345330.174345016</v>
+      </c>
+      <c r="D36" s="62">
+        <v>1</v>
+      </c>
+      <c r="E36" s="62">
+        <v>0</v>
+      </c>
+      <c r="F36" s="62">
+        <v>0</v>
+      </c>
+      <c r="G36" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="62">
+        <v>0.83</v>
+      </c>
+      <c r="I36" s="62">
+        <v>0</v>
+      </c>
+      <c r="J36" s="62">
+        <v>1</v>
+      </c>
+      <c r="K36" s="62">
+        <v>0</v>
+      </c>
+      <c r="L36" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M36" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N36" s="62">
+        <v>0</v>
+      </c>
+      <c r="O36" s="62">
+        <v>0</v>
+      </c>
+      <c r="P36" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="62">
+        <v>1</v>
+      </c>
+      <c r="R36" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A23:A36">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>